<commit_message>
Some changes on the files
</commit_message>
<xml_diff>
--- a/zzyTest/Customer.xlsx
+++ b/zzyTest/Customer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\isem2006\ISEM_Grop_proj\zzyTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LYLJack\Desktop\isemGroupProject\Version2\ISEM_Grop_proj-master\ISEM_Grop_proj\zzyTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C542088-9CBE-478A-8792-49D0F4EF612B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02AB19B-2254-473C-A6A1-0957C56C4498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,64 +43,101 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Cust1Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cust2Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cust3Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cust4Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HKBUClassRoom1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HKBUClassRoom2</t>
-  </si>
-  <si>
-    <t>HKBUClassRoom3</t>
-  </si>
-  <si>
-    <t>HKBUClassRoom4</t>
-  </si>
-  <si>
-    <t>Cust5Name</t>
-  </si>
-  <si>
-    <t>HKBUClassRoom5</t>
-  </si>
-  <si>
-    <t>Cust6Name</t>
-  </si>
-  <si>
-    <t>HKBUClassRoom6</t>
-  </si>
-  <si>
-    <t>Cust7Name</t>
-  </si>
-  <si>
-    <t>HKBUClassRoom7</t>
-  </si>
-  <si>
-    <t>Cust8Name</t>
-  </si>
-  <si>
-    <t>HKBUClassRoom8</t>
+    <t>Tristan Dungey</t>
+  </si>
+  <si>
+    <t>PO Box 68312</t>
+  </si>
+  <si>
+    <t>Teresa Bremner</t>
+  </si>
+  <si>
+    <t>PO Box 3088</t>
+  </si>
+  <si>
+    <t>Mureil Antoons</t>
+  </si>
+  <si>
+    <t>PO Box 13897</t>
+  </si>
+  <si>
+    <t>Xerxes Pierucci</t>
+  </si>
+  <si>
+    <t>Suite 8</t>
+  </si>
+  <si>
+    <t>Isaak Simoneschi</t>
+  </si>
+  <si>
+    <t>Suite 71</t>
+  </si>
+  <si>
+    <t>Dirk Toffel</t>
+  </si>
+  <si>
+    <t>PO Box 97328</t>
+  </si>
+  <si>
+    <t>Bianka Pendre</t>
+  </si>
+  <si>
+    <t>PO Box 91677</t>
+  </si>
+  <si>
+    <t>Tamarra Akenhead</t>
+  </si>
+  <si>
+    <t>Suite 36</t>
+  </si>
+  <si>
+    <t>Dotty Guilloneau</t>
+  </si>
+  <si>
+    <t>10th Floor</t>
+  </si>
+  <si>
+    <t>Kayle Lambole</t>
+  </si>
+  <si>
+    <t>Suite 9</t>
+  </si>
+  <si>
+    <t>Bev Trevna</t>
+  </si>
+  <si>
+    <t>Apt 1564</t>
+  </si>
+  <si>
+    <t>Evelyn Powers</t>
+  </si>
+  <si>
+    <t>17th Floor</t>
+  </si>
+  <si>
+    <t>Eugene Belamy</t>
+  </si>
+  <si>
+    <t>PO Box 48352</t>
+  </si>
+  <si>
+    <t>Mel Bernardo</t>
+  </si>
+  <si>
+    <t>Suite 81</t>
+  </si>
+  <si>
+    <t>Collin Mandy</t>
+  </si>
+  <si>
+    <t>9th Floor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +147,18 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -133,14 +182,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Normal" xfId="2" xr:uid="{9C3E6293-49A9-4E15-BD3F-9DDD516362DF}"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 2" xfId="1" xr:uid="{053D639F-A361-4E53-9B37-E82DCB7BB744}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -418,20 +472,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="3" width="19.4140625" customWidth="1"/>
-    <col min="4" max="4" width="13.75" customWidth="1"/>
+    <col min="2" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,12 +499,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C2">
         <v>987654</v>
@@ -459,102 +513,200 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>111001</v>
+        <v>114514</v>
       </c>
       <c r="D3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>298732</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
-        <v>111002</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5">
-        <v>111003</v>
+        <v>586324</v>
       </c>
       <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C6">
-        <v>111004</v>
+        <v>755219</v>
       </c>
       <c r="D6">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C7">
-        <v>111005</v>
+        <v>458820</v>
       </c>
       <c r="D7">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C8">
-        <v>111006</v>
+        <v>879624</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C9">
-        <v>111007</v>
+        <v>314778</v>
       </c>
       <c r="D9">
         <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>412789</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>203578</v>
+      </c>
+      <c r="D11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>155985</v>
+      </c>
+      <c r="D12">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>984203</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>741265</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15">
+        <v>354154</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16">
+        <v>654523</v>
+      </c>
+      <c r="D16">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>